<commit_message>
Finished testing doc for Sprint 1, fixes need to be made
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\4thYear\EPL449\epl343.winter18.team10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHRISIS-PC\Desktop\8th Semester\EPL449\epl343.winter18.team10\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3753FDB0-D0CE-40A0-B0E6-67E2C099153B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
   <si>
     <t>User Story</t>
   </si>
@@ -140,16 +141,94 @@
     <t>Application runs and after selecting 'Invoice' in the side menu and 'Create' in the top bar menu you can select the Customer, adjust his info, select Products, adjust their prices/quantity and by pressing Complete send the information to the Database.</t>
   </si>
   <si>
-    <t>No validations in Quantity and Price for negative values</t>
-  </si>
-  <si>
     <t>Awaiting Fix</t>
+  </si>
+  <si>
+    <t>Application runs and after selecting 'Invoice' in the side menu and 'Edit' in the top bar menu and then insert the Invoice ID in the corresponding text box, all the invoice's details including customer information and products are displayed in their corresponding elements and then you can edit the products information.</t>
+  </si>
+  <si>
+    <t>No check in Quantity and Price for negative values
+Duplicate products should not be allowed</t>
+  </si>
+  <si>
+    <t>No check in Quantity and Price for negative values
+Duplicate products should not be allowed
+When an invoice is already loaded, pressing load again will not clear previous invoice</t>
+  </si>
+  <si>
+    <t>Awaiting Fix
+(Fixed loading new invocie)</t>
+  </si>
+  <si>
+    <t>1, 3</t>
+  </si>
+  <si>
+    <t>Application runs and after selecting 'Invoice' in the side menu and 'View' in the top bar menu and then insert the Invoice ID in the corresponding text box, all the invoice's details are loaded and when you press print then  Adobe Acrobat Reader runs with the print dialog window open</t>
+  </si>
+  <si>
+    <t>No check if an invoice is loaded or not.</t>
+  </si>
+  <si>
+    <t>No check if an invoice is loaded or not.
+The temp pdf is not removed afterwards</t>
+  </si>
+  <si>
+    <t>Application runs and after selecting 'Invoice' in the side menu and 'View' in the top bar menu and then insert the Invoice ID in the corresponding text box, all the invoice's details are loaded and when you press save then the invoice is saved in the predetermined location.</t>
+  </si>
+  <si>
+    <t>Application runs and after selecting 'Invoice' in the side menu and 'View' in the top bar menu and then insert the Invoice ID in the corresponding text box, all the invoice's details are loaded and when you press preview then Adobe Acrobat Reader and displays the pdf to be created.</t>
+  </si>
+  <si>
+    <t>Application runs and after selecting 'Customers' in the side menu and 'View' in the top bar menu you can see all the customers from the Database, in a grid. You can also filter results by Balance, Customer name and City.</t>
+  </si>
+  <si>
+    <t>Application runs and after selecting 'Customers' in the side menu and 'Create' in the top bar menu you can add all the information you need to create a new customer and then press Create to complete.</t>
+  </si>
+  <si>
+    <t>No email and phone number validations</t>
+  </si>
+  <si>
+    <t>Application runs and after selecting 'Customers' in the side menu and 'Edit' in the top bar menu and load the customer you want you can  edit all his information then press Update to complete.</t>
+  </si>
+  <si>
+    <t>Cannot remove customers that are referenced in the Database as that violated the foreign keys constraints</t>
+  </si>
+  <si>
+    <t>Application runs and after selecting 'Customers' in the side menu and View in the top bar menu you can see all the customers from the Database, in a grid and by selecting Delete from the options on the right the customer is removed.</t>
+  </si>
+  <si>
+    <t>Application runs and after selecting 'Product' in the side menu and Create in the top bar menu you can add all the information of a product in the textboxes and then complete with the Create button.</t>
+  </si>
+  <si>
+    <t>No check in most text boxes for negative values
+(price, cost, stock)</t>
+  </si>
+  <si>
+    <t>Application runs and after selecting 'Product' in the side menu and 'View' in the top bar menu you can see all the products from the Database, in a grid. You can also filter results by Category, Product name and Status.</t>
+  </si>
+  <si>
+    <t>Application runs and after selecting 'Product' in the side menu and 'Edit' in the top bar menu and load the product you want you can  edit all its information then press Update to complete.</t>
+  </si>
+  <si>
+    <t>No check in most text boxes for negative values
+(price, cost, stock)
+No validation for VAT</t>
+  </si>
+  <si>
+    <t>Application runs and after selecting 'Settings' in the side menu you can load all the users/ remove users and add new users</t>
+  </si>
+  <si>
+    <t>As expected
+(but its ugly)</t>
+  </si>
+  <si>
+    <t>Awaiting Beautyfication</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -291,14 +370,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -317,9 +393,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -338,17 +411,26 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -633,20 +715,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="46" style="8" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="47.140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="46" style="7" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="47.140625" style="9" customWidth="1"/>
     <col min="6" max="6" width="24" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -655,375 +737,505 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+      <c r="A3" s="17">
         <v>1</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="12">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="10">
         <v>43896</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="15" t="s">
+      <c r="H3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="14">
+      <c r="A4" s="17"/>
+      <c r="B4" s="12">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="14">
         <v>1</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="10">
         <v>43896</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="15" t="s">
+      <c r="H4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="14">
+      <c r="A5" s="17"/>
+      <c r="B5" s="12">
         <v>3</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="10">
         <v>43896</v>
       </c>
-      <c r="H5" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="15" t="s">
+      <c r="H5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="14">
+      <c r="A6" s="17"/>
+      <c r="B6" s="12">
         <v>4</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="14">
         <v>1</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="10">
+        <v>43897</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="12">
-        <v>43897</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="19" t="s">
+    </row>
+    <row r="7" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="12">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="14">
-        <v>5</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="14">
+      <c r="F7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="10">
+        <v>43898</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="12">
         <v>6</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="14">
+      <c r="D8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="10">
+        <v>43898</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="12">
         <v>7</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="14">
+      <c r="D9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="10">
+        <v>43898</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="12">
         <v>8</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="14">
+      <c r="D10" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="10">
+        <v>43898</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="17"/>
+      <c r="B11" s="12">
         <v>9</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="14">
         <v>1</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="14">
+      <c r="E11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="10">
+        <v>43898</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="12">
         <v>10</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="14">
         <v>1</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="14">
+      <c r="E12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="10">
+        <v>43898</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="12">
         <v>11</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="14">
+      <c r="E13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="10">
+        <v>43898</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="12">
         <v>12</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="14">
+      <c r="E14" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="10">
+        <v>43898</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="12">
         <v>13</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="14">
         <v>1</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="14">
+      <c r="E15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="10">
+        <v>43898</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="12">
         <v>14</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="14">
         <v>1</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="14">
+      <c r="E16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="10">
+        <v>43898</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="12">
         <v>15</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="14">
+      <c r="E17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="10">
+        <v>43898</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="12">
         <v>16</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="E18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="10">
+        <v>43898</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="14">
+      <c r="A19" s="17"/>
+      <c r="B19" s="12">
         <v>17</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="14">
         <v>1</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="E19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="10">
+        <v>43898</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>